<commit_message>
Session 28: Regression tests passed, Empleado demo page created
- All 3 regression tests passed (features #15, #114, #7)
- Created /demo/empleado page for testing Empleado sidebar navigation
- 6 features skipped (backend required)
- Feature stats: 119/157 (75.8%) complete

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/.playwright-mcp/reporte-mdayuda-2026-01-07.xlsx
+++ b/.playwright-mcp/reporte-mdayuda-2026-01-07.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -417,85 +417,80 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Generado: 7 de enero de 2026, 7:43</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Filtro aplicado: Sistema de Ventas</v>
+        <v>Generado: 7 de enero de 2026, 18:03</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Resumen General de Tickets</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Resumen General de Tickets</v>
+        <v>Estado</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Cantidad</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Estado</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Cantidad</v>
+        <v>Total de Tickets</v>
+      </c>
+      <c r="B6">
+        <v>156</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Total de Tickets</v>
+        <v>Abiertos</v>
       </c>
       <c r="B7">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Abiertos</v>
+        <v>En Proceso</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>En Proceso</v>
+        <v>En Espera</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>En Espera</v>
+        <v>Resueltos</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Resueltos</v>
+        <v>Cerrados</v>
       </c>
       <c r="B11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Cerrados</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B11"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,9 +527,64 @@
         <v>28.8%</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Portal Web</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4" t="str">
+        <v>20.5%</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Aplicacion Movil</v>
+      </c>
+      <c r="B5">
+        <v>28</v>
+      </c>
+      <c r="C5" t="str">
+        <v>17.9%</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Sistema de Inventario</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6" t="str">
+        <v>15.4%</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Facturacion</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7" t="str">
+        <v>9.6%</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Otros</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8" t="str">
+        <v>7.7%</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -572,7 +622,7 @@
         <v>Alta</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C3" t="str">
         <v>24.4%</v>
@@ -583,7 +633,7 @@
         <v>Media</v>
       </c>
       <c r="B4">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="C4" t="str">
         <v>50%</v>
@@ -594,7 +644,7 @@
         <v>Baja</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C5" t="str">
         <v>25.6%</v>
@@ -609,7 +659,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -653,9 +703,65 @@
         <v>95%</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Carlos Rodriguez</v>
+      </c>
+      <c r="B4">
+        <v>38</v>
+      </c>
+      <c r="C4" t="str">
+        <v>5.1 horas</v>
+      </c>
+      <c r="D4" t="str">
+        <v>92%</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Ana Martinez</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5" t="str">
+        <v>3.8 horas</v>
+      </c>
+      <c r="D5" t="str">
+        <v>98%</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Luis Fernandez</v>
+      </c>
+      <c r="B6">
+        <v>28</v>
+      </c>
+      <c r="C6" t="str">
+        <v>6.2 horas</v>
+      </c>
+      <c r="D6" t="str">
+        <v>88%</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Sofia Torres</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7" t="str">
+        <v>4.5 horas</v>
+      </c>
+      <c r="D7" t="str">
+        <v>91%</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -689,7 +795,7 @@
         <v>Tickets con SLA Cumplido</v>
       </c>
       <c r="B3">
-        <v>41</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4">
@@ -697,7 +803,7 @@
         <v>Tickets con SLA Incumplido</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">

</xml_diff>